<commit_message>
the Accurcay and forecasts file
</commit_message>
<xml_diff>
--- a/LinearRegression_Accuracy.xlsx
+++ b/LinearRegression_Accuracy.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,156 +434,38 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>3</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Train RMSE</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Test RMSE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Train MAE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Test MAE</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>804.1864288928817</v>
+        <v>804.1864288928818</v>
       </c>
       <c r="B2" t="n">
-        <v>543.7011417795203</v>
+        <v>543.7011417795202</v>
       </c>
       <c r="C2" t="n">
-        <v>530.3719787638132</v>
+        <v>530.3719787638131</v>
       </c>
       <c r="D2" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B3" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C3" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D3" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B4" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C4" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D4" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B5" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C5" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D5" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B6" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C6" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D6" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B7" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C7" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D7" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B8" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C8" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D8" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B9" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C9" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D9" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B10" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C10" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D10" t="n">
-        <v>440.053699993206</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>804.1864288928817</v>
-      </c>
-      <c r="B11" t="n">
-        <v>543.7011417795203</v>
-      </c>
-      <c r="C11" t="n">
-        <v>530.3719787638132</v>
-      </c>
-      <c r="D11" t="n">
         <v>440.053699993206</v>
       </c>
     </row>

</xml_diff>